<commit_message>
final change at time testing celery
</commit_message>
<xml_diff>
--- a/codezen/celeryProduct/static/excel/Product_data.xlsx
+++ b/codezen/celeryProduct/static/excel/Product_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t xml:space="preserve">product_name</t>
   </si>
@@ -28,16 +28,127 @@
     <t xml:space="preserve">amount</t>
   </si>
   <si>
-    <t xml:space="preserve">ram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdwskjfd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">samosa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sampo</t>
+    <t xml:space="preserve">RONEMOX 250MG - GY CAPSULE 10S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RONEMOX 250MG CAPSULES 10’S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAFEROXIM 500 TABLET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMOXYCLAV DRY SYRUP 30ML HDPE BOTTLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABBOTT GRIPE WATER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZITHROLECT 250 TABS 6S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMOXYCLAV 375 MG TABLETS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCABIGARD 100ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAFEXIM 100 TABLET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZITHROLECT 500 TABS 3S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAFEXIM 200 TABLET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHENSEDYL DX 60 ML SYRUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCABIGARD-P LOTION 50ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCAL TABLETS 15S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB-ROZU 5 TABLETS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NKACIN 500MG INJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUPERQUIN 500MG TABLETS 5S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMOXYCLAV 1GM TABLET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHUPP 60ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECABOLIN 50 - 1ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEWCOLD ML TABLETS 10S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RONEMOX 500 CAPS 10S Y/Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAFEPODOX 100MG DT10S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABTELMI 20 TABLETS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RZOLE LSR CAPSULES 10S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHENSEDYL DX SYRUP 100ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROGRO SYRUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMBULIDE 100 (BLUE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C ONE 500MG INJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C ONE INJECTION 250MG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NICOPENTA INJECTION CLEAR VIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABAMLO 5 TABLETS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NICOFLOX 200MG TAB 10S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIRACIT TABS 10MG 10S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICLOFAM GEL 30 G TUBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCLOPID 75 TABLETS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABETOROX 120 TABLETS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABETOROX 90 TABLETS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB-GLYMPRD M 1 TABLETS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB-GLYMPRD M 2 TABLETS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABIXIM 100MG TAB 10S</t>
   </si>
 </sst>
 </file>
@@ -52,7 +163,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -134,13 +244,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -159,7 +269,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>23423</v>
+        <v>9375</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -167,7 +277,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>2342</v>
+        <v>9375</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -175,7 +285,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>23458</v>
+        <v>19638</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -183,7 +293,367 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>252</v>
+        <v>10400</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>41040</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>18560</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>6840</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>19980</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>16250</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>46913</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>9520</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>24600</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>34200</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>3270</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>3375</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>23500</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>7600</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>2790</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>16300</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>57500</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>79920</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>34200</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>15600</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>2970</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>1225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>